<commit_message>
adding images for ML report
</commit_message>
<xml_diff>
--- a/ML/2020_tests/2020_draft_model_testing.xlsx
+++ b/ML/2020_tests/2020_draft_model_testing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brady\Desktop\1_BootcampProjects\final_project\NBA_draft_analysis\ML\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brady\Desktop\1_BootcampProjects\final_project\NBA_draft_analysis\ML\2020_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5BA291-7152-49A1-96BD-741A6A91639C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F7DDF1-EAE4-4956-B8BB-DCE27E7B697B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{65649B7E-C7DD-4EBF-BF5F-B4B5EA2BB1C0}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{65649B7E-C7DD-4EBF-BF5F-B4B5EA2BB1C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -234,7 +234,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -300,6 +300,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -623,7 +626,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomRight" activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -632,13 +635,13 @@
     <col min="4" max="4" width="11.3671875" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.41796875" style="5" customWidth="1"/>
     <col min="6" max="6" width="7.05078125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="8.26171875" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.68359375" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="3.68359375" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.68359375" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.05078125" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.47265625" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.68359375" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.26171875" style="11" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="4.68359375" style="5" hidden="1" customWidth="1"/>
+    <col min="9" max="10" width="3.68359375" style="5" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="4.68359375" style="5" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="8.05078125" style="9" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="5.47265625" style="9" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="6.68359375" style="9" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="8.26171875" style="11" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4.68359375" style="5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="3.68359375" style="5" bestFit="1" customWidth="1"/>
@@ -835,18 +838,18 @@
         <v>0.12</v>
       </c>
       <c r="W3" s="7">
-        <f t="shared" ref="W3:W40" si="0">P3/(P3+R3)</f>
+        <f>P3/(P3+R3)</f>
         <v>0.99794520547945209</v>
       </c>
       <c r="X3" s="7">
-        <f t="shared" ref="X3:X40" si="1">P3/(P3+Q3)</f>
+        <f>P3/(P3+Q3)</f>
         <v>0.7429882712901581</v>
       </c>
       <c r="Y3" s="18">
         <v>10</v>
       </c>
       <c r="Z3" s="7">
-        <f t="shared" ref="Z3:Z40" si="2">Y3/39</f>
+        <f>Y3/39</f>
         <v>0.25641025641025639</v>
       </c>
     </row>
@@ -918,23 +921,23 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="W4" s="7">
-        <f t="shared" si="0"/>
+        <f>P4/(P4+R4)</f>
         <v>0.99637681159420288</v>
       </c>
       <c r="X4" s="7">
-        <f t="shared" si="1"/>
+        <f>P4/(P4+Q4)</f>
         <v>0.56093829678735341</v>
       </c>
       <c r="Y4" s="18">
         <v>4</v>
       </c>
       <c r="Z4" s="7">
-        <f t="shared" si="2"/>
+        <f>Y4/39</f>
         <v>0.10256410256410256</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="23" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="5">
@@ -998,23 +1001,23 @@
         <v>0.12</v>
       </c>
       <c r="W5" s="7">
-        <f t="shared" si="0"/>
+        <f>P5/(P5+R5)</f>
         <v>0.99655647382920109</v>
       </c>
       <c r="X5" s="7">
-        <f t="shared" si="1"/>
+        <f>P5/(P5+Q5)</f>
         <v>0.73788883222845492</v>
       </c>
       <c r="Y5" s="18">
         <v>9</v>
       </c>
       <c r="Z5" s="7">
-        <f t="shared" si="2"/>
+        <f>Y5/39</f>
         <v>0.23076923076923078</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="23" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="5">
@@ -1078,24 +1081,24 @@
         <v>0.16</v>
       </c>
       <c r="W6" s="7">
-        <f t="shared" si="0"/>
+        <f>P6/(P6+R6)</f>
         <v>0.99296187683284454</v>
       </c>
       <c r="X6" s="7">
-        <f t="shared" si="1"/>
+        <f>P6/(P6+Q6)</f>
         <v>0.86333503314635385</v>
       </c>
       <c r="Y6" s="18">
         <v>8</v>
       </c>
       <c r="Z6" s="7">
-        <f t="shared" si="2"/>
+        <f>Y6/39</f>
         <v>0.20512820512820512</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="5" t="s">
-        <v>23</v>
+      <c r="A7" s="23" t="s">
+        <v>12</v>
       </c>
       <c r="B7" s="5">
         <v>0.25</v>
@@ -1104,46 +1107,46 @@
         <v>22</v>
       </c>
       <c r="D7" s="5">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G7" s="11">
-        <v>0.90400000000000003</v>
+        <v>0.86050000000000004</v>
       </c>
       <c r="H7" s="5">
-        <v>5066</v>
+        <v>122</v>
       </c>
       <c r="I7" s="5">
-        <v>637</v>
+        <v>27</v>
       </c>
       <c r="J7" s="5">
-        <v>512</v>
+        <v>14</v>
       </c>
       <c r="K7" s="5">
-        <v>5748</v>
+        <v>131</v>
       </c>
       <c r="L7" s="9">
+        <v>0.83</v>
+      </c>
+      <c r="M7" s="9">
         <v>0.9</v>
       </c>
-      <c r="M7" s="9">
-        <v>0.92</v>
-      </c>
       <c r="N7" s="9">
-        <v>0.91</v>
+        <v>0.86</v>
       </c>
       <c r="O7" s="11">
-        <v>0.86050000000000004</v>
+        <v>0.86599999999999999</v>
       </c>
       <c r="P7" s="5">
-        <v>1695</v>
+        <v>1706</v>
       </c>
       <c r="Q7" s="5">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="R7" s="5">
         <v>13</v>
@@ -1161,23 +1164,23 @@
         <v>0.16</v>
       </c>
       <c r="W7" s="7">
-        <f t="shared" si="0"/>
-        <v>0.99238875878220145</v>
+        <f>P7/(P7+R7)</f>
+        <v>0.99243746364165208</v>
       </c>
       <c r="X7" s="7">
-        <f t="shared" si="1"/>
-        <v>0.86435492095869459</v>
+        <f>P7/(P7+Q7)</f>
+        <v>0.86996430392656809</v>
       </c>
       <c r="Y7" s="18">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="Z7" s="7">
-        <f t="shared" si="2"/>
-        <v>0.20512820512820512</v>
+        <f>Y7/39</f>
+        <v>0.17948717948717949</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="23" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="5">
@@ -1187,7 +1190,7 @@
         <v>22</v>
       </c>
       <c r="D8" s="5">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>17</v>
@@ -1196,19 +1199,19 @@
         <v>16</v>
       </c>
       <c r="G8" s="11">
-        <v>0.90369999999999995</v>
+        <v>0.90400000000000003</v>
       </c>
       <c r="H8" s="5">
-        <v>5067</v>
+        <v>5066</v>
       </c>
       <c r="I8" s="5">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="J8" s="5">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="K8" s="5">
-        <v>5744</v>
+        <v>5748</v>
       </c>
       <c r="L8" s="9">
         <v>0.9</v>
@@ -1220,13 +1223,13 @@
         <v>0.91</v>
       </c>
       <c r="O8" s="11">
-        <v>0.86</v>
+        <v>0.86050000000000004</v>
       </c>
       <c r="P8" s="5">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="Q8" s="5">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="R8" s="5">
         <v>13</v>
@@ -1244,24 +1247,24 @@
         <v>0.16</v>
       </c>
       <c r="W8" s="7">
-        <f t="shared" si="0"/>
-        <v>0.99238429994141775</v>
+        <f>P8/(P8+R8)</f>
+        <v>0.99238875878220145</v>
       </c>
       <c r="X8" s="7">
-        <f t="shared" si="1"/>
-        <v>0.86384497705252428</v>
+        <f>P8/(P8+Q8)</f>
+        <v>0.86435492095869459</v>
       </c>
       <c r="Y8" s="18">
         <v>8</v>
       </c>
       <c r="Z8" s="7">
-        <f t="shared" si="2"/>
+        <f>Y8/39</f>
         <v>0.20512820512820512</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="5" t="s">
-        <v>12</v>
+      <c r="A9" s="23" t="s">
+        <v>23</v>
       </c>
       <c r="B9" s="5">
         <v>0.25</v>
@@ -1273,43 +1276,43 @@
         <v>10000</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="11">
-        <v>0.86050000000000004</v>
+        <v>0.90369999999999995</v>
       </c>
       <c r="H9" s="5">
-        <v>122</v>
+        <v>5067</v>
       </c>
       <c r="I9" s="5">
-        <v>27</v>
+        <v>636</v>
       </c>
       <c r="J9" s="5">
-        <v>14</v>
+        <v>516</v>
       </c>
       <c r="K9" s="5">
-        <v>131</v>
+        <v>5744</v>
       </c>
       <c r="L9" s="9">
-        <v>0.83</v>
+        <v>0.9</v>
       </c>
       <c r="M9" s="9">
-        <v>0.9</v>
+        <v>0.92</v>
       </c>
       <c r="N9" s="9">
+        <v>0.91</v>
+      </c>
+      <c r="O9" s="11">
         <v>0.86</v>
       </c>
-      <c r="O9" s="11">
-        <v>0.86599999999999999</v>
-      </c>
       <c r="P9" s="5">
-        <v>1706</v>
+        <v>1694</v>
       </c>
       <c r="Q9" s="5">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="R9" s="5">
         <v>13</v>
@@ -1327,23 +1330,23 @@
         <v>0.16</v>
       </c>
       <c r="W9" s="7">
-        <f t="shared" si="0"/>
-        <v>0.99243746364165208</v>
+        <f>P9/(P9+R9)</f>
+        <v>0.99238429994141775</v>
       </c>
       <c r="X9" s="7">
-        <f t="shared" si="1"/>
-        <v>0.86996430392656809</v>
+        <f>P9/(P9+Q9)</f>
+        <v>0.86384497705252428</v>
       </c>
       <c r="Y9" s="18">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Z9" s="7">
-        <f t="shared" si="2"/>
-        <v>0.17948717948717949</v>
+        <f>Y9/39</f>
+        <v>0.20512820512820512</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="23" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="5">
@@ -1410,23 +1413,23 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="W10" s="7">
-        <f t="shared" si="0"/>
+        <f>P10/(P10+R10)</f>
         <v>0.99165175909361958</v>
       </c>
       <c r="X10" s="7">
-        <f t="shared" si="1"/>
+        <f>P10/(P10+Q10)</f>
         <v>0.8480367159612443</v>
       </c>
       <c r="Y10" s="18">
         <v>7</v>
       </c>
       <c r="Z10" s="7">
-        <f t="shared" si="2"/>
+        <f>Y10/39</f>
         <v>0.17948717948717949</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="23" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="5">
@@ -1490,23 +1493,23 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="W11" s="7">
-        <f t="shared" si="0"/>
+        <f>P11/(P11+R11)</f>
         <v>0.99164677804295942</v>
       </c>
       <c r="X11" s="7">
-        <f t="shared" si="1"/>
+        <f>P11/(P11+Q11)</f>
         <v>0.84752677205507398</v>
       </c>
       <c r="Y11" s="18">
         <v>7</v>
       </c>
       <c r="Z11" s="7">
-        <f t="shared" si="2"/>
+        <f>Y11/39</f>
         <v>0.17948717948717949</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="23" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="5">
@@ -1570,33 +1573,33 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="W12" s="7">
-        <f t="shared" si="0"/>
+        <f>P12/(P12+R12)</f>
         <v>0.99164179104477612</v>
       </c>
       <c r="X12" s="7">
-        <f t="shared" si="1"/>
+        <f>P12/(P12+Q12)</f>
         <v>0.84701682814890367</v>
       </c>
       <c r="Y12" s="18">
         <v>7</v>
       </c>
       <c r="Z12" s="7">
-        <f t="shared" si="2"/>
+        <f>Y12/39</f>
         <v>0.17948717948717949</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>22</v>
+        <v>0.05</v>
+      </c>
+      <c r="C13" s="5">
+        <v>10</v>
       </c>
       <c r="D13" s="5">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>19</v>
@@ -1605,37 +1608,37 @@
         <v>16</v>
       </c>
       <c r="G13" s="11">
-        <v>0.83399999999999996</v>
+        <v>0.79659999999999997</v>
       </c>
       <c r="H13" s="5">
-        <v>123</v>
+        <v>20</v>
       </c>
       <c r="I13" s="5">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="J13" s="5">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="K13" s="5">
-        <v>131</v>
+        <v>27</v>
       </c>
       <c r="L13" s="9">
-        <v>0.83</v>
+        <v>0.84</v>
       </c>
       <c r="M13" s="9">
-        <v>0.9</v>
+        <v>0.79</v>
       </c>
       <c r="N13" s="9">
-        <v>0.87</v>
+        <v>0.82</v>
       </c>
       <c r="O13" s="11">
-        <v>0.86650000000000005</v>
+        <v>0.89849999999999997</v>
       </c>
       <c r="P13" s="5">
-        <v>1709</v>
+        <v>1773</v>
       </c>
       <c r="Q13" s="5">
-        <v>252</v>
+        <v>188</v>
       </c>
       <c r="R13" s="5">
         <v>15</v>
@@ -1644,32 +1647,32 @@
         <v>24</v>
       </c>
       <c r="T13" s="9">
-        <v>0.09</v>
+        <v>0.11</v>
       </c>
       <c r="U13" s="9">
         <v>0.62</v>
       </c>
       <c r="V13" s="9">
-        <v>0.15</v>
+        <v>0.19</v>
       </c>
       <c r="W13" s="7">
-        <f t="shared" si="0"/>
-        <v>0.99129930394431554</v>
+        <f>P13/(P13+R13)</f>
+        <v>0.99161073825503354</v>
       </c>
       <c r="X13" s="7">
-        <f t="shared" si="1"/>
-        <v>0.87149413564507905</v>
+        <f>P13/(P13+Q13)</f>
+        <v>0.90413054563997963</v>
       </c>
       <c r="Y13" s="18">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="Z13" s="7">
-        <f t="shared" si="2"/>
-        <v>0.20512820512820512</v>
+        <f>Y13/39</f>
+        <v>0.15384615384615385</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="5">
@@ -1736,33 +1739,33 @@
         <v>0.15</v>
       </c>
       <c r="W14" s="7">
-        <f t="shared" si="0"/>
+        <f>P14/(P14+R14)</f>
         <v>0.99131441806601039</v>
       </c>
       <c r="X14" s="7">
-        <f t="shared" si="1"/>
+        <f>P14/(P14+Q14)</f>
         <v>0.87302396736359</v>
       </c>
       <c r="Y14" s="18">
         <v>7</v>
       </c>
       <c r="Z14" s="7">
-        <f t="shared" si="2"/>
+        <f>Y14/39</f>
         <v>0.17948717948717949</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="C15" s="5">
-        <v>10</v>
+        <v>0.25</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="D15" s="5">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>19</v>
@@ -1771,37 +1774,37 @@
         <v>16</v>
       </c>
       <c r="G15" s="11">
-        <v>0.79659999999999997</v>
+        <v>0.83399999999999996</v>
       </c>
       <c r="H15" s="5">
-        <v>20</v>
+        <v>123</v>
       </c>
       <c r="I15" s="5">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="J15" s="5">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="K15" s="5">
-        <v>27</v>
+        <v>131</v>
       </c>
       <c r="L15" s="9">
-        <v>0.84</v>
+        <v>0.83</v>
       </c>
       <c r="M15" s="9">
-        <v>0.79</v>
+        <v>0.9</v>
       </c>
       <c r="N15" s="9">
-        <v>0.82</v>
+        <v>0.87</v>
       </c>
       <c r="O15" s="11">
-        <v>0.89849999999999997</v>
+        <v>0.86650000000000005</v>
       </c>
       <c r="P15" s="5">
-        <v>1773</v>
+        <v>1709</v>
       </c>
       <c r="Q15" s="5">
-        <v>188</v>
+        <v>252</v>
       </c>
       <c r="R15" s="5">
         <v>15</v>
@@ -1810,32 +1813,32 @@
         <v>24</v>
       </c>
       <c r="T15" s="9">
-        <v>0.11</v>
+        <v>0.09</v>
       </c>
       <c r="U15" s="9">
         <v>0.62</v>
       </c>
       <c r="V15" s="9">
-        <v>0.19</v>
+        <v>0.15</v>
       </c>
       <c r="W15" s="7">
-        <f t="shared" si="0"/>
-        <v>0.99161073825503354</v>
+        <f>P15/(P15+R15)</f>
+        <v>0.99129930394431554</v>
       </c>
       <c r="X15" s="7">
-        <f t="shared" si="1"/>
-        <v>0.90413054563997963</v>
+        <f>P15/(P15+Q15)</f>
+        <v>0.87149413564507905</v>
       </c>
       <c r="Y15" s="18">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Z15" s="7">
-        <f t="shared" si="2"/>
-        <v>0.15384615384615385</v>
+        <f>Y15/39</f>
+        <v>0.20512820512820512</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="5">
@@ -1902,29 +1905,32 @@
         <v>0.16</v>
       </c>
       <c r="W16" s="7">
-        <f t="shared" si="0"/>
+        <f>P16/(P16+R16)</f>
         <v>0.99086236436322106</v>
       </c>
       <c r="X16" s="7">
-        <f t="shared" si="1"/>
+        <f>P16/(P16+Q16)</f>
         <v>0.88475267720550743</v>
       </c>
       <c r="Y16" s="18">
         <v>7</v>
       </c>
       <c r="Z16" s="7">
-        <f t="shared" si="2"/>
+        <f>Y16/39</f>
         <v>0.17948717948717949</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="5" t="s">
-        <v>26</v>
+      <c r="A17" s="23" t="s">
+        <v>12</v>
       </c>
       <c r="B17" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="C17" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="5">
         <v>10</v>
       </c>
       <c r="E17" s="5" t="s">
@@ -1934,37 +1940,37 @@
         <v>16</v>
       </c>
       <c r="G17" s="11">
-        <v>0.86439999999999995</v>
+        <v>0.83299999999999996</v>
       </c>
       <c r="H17" s="5">
+        <v>120</v>
+      </c>
+      <c r="I17" s="5">
+        <v>29</v>
+      </c>
+      <c r="J17" s="5">
         <v>20</v>
       </c>
-      <c r="I17" s="5">
-        <v>5</v>
-      </c>
-      <c r="J17" s="5">
-        <v>3</v>
-      </c>
       <c r="K17" s="5">
-        <v>31</v>
+        <v>125</v>
       </c>
       <c r="L17" s="9">
+        <v>0.81</v>
+      </c>
+      <c r="M17" s="9">
         <v>0.86</v>
       </c>
-      <c r="M17" s="9">
-        <v>0.91</v>
-      </c>
       <c r="N17" s="9">
-        <v>0.89</v>
+        <v>0.84</v>
       </c>
       <c r="O17" s="11">
-        <v>0.874</v>
+        <v>0.88300000000000001</v>
       </c>
       <c r="P17" s="5">
-        <v>1726</v>
+        <v>1744</v>
       </c>
       <c r="Q17" s="5">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="R17" s="5">
         <v>17</v>
@@ -1979,26 +1985,26 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="V17" s="9">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="W17" s="7">
-        <f t="shared" si="0"/>
-        <v>0.99024670109007462</v>
+        <f>P17/(P17+R17)</f>
+        <v>0.99034639409426461</v>
       </c>
       <c r="X17" s="7">
-        <f t="shared" si="1"/>
-        <v>0.88016318204997446</v>
+        <f>P17/(P17+Q17)</f>
+        <v>0.8893421723610403</v>
       </c>
       <c r="Y17" s="18">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="Z17" s="7">
-        <f t="shared" si="2"/>
-        <v>0.17948717948717949</v>
+        <f>Y17/39</f>
+        <v>0.10256410256410256</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="23" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="5">
@@ -2065,32 +2071,29 @@
         <v>0.15</v>
       </c>
       <c r="W18" s="7">
-        <f t="shared" si="0"/>
+        <f>P18/(P18+R18)</f>
         <v>0.99029126213592233</v>
       </c>
       <c r="X18" s="7">
-        <f t="shared" si="1"/>
+        <f>P18/(P18+Q18)</f>
         <v>0.88424273329933711</v>
       </c>
       <c r="Y18" s="18">
         <v>5</v>
       </c>
       <c r="Z18" s="7">
-        <f t="shared" si="2"/>
+        <f>Y18/39</f>
         <v>0.12820512820512819</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="5" t="s">
-        <v>12</v>
+      <c r="A19" s="23" t="s">
+        <v>26</v>
       </c>
       <c r="B19" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="C19" s="5">
         <v>10</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -2100,37 +2103,37 @@
         <v>16</v>
       </c>
       <c r="G19" s="11">
-        <v>0.83299999999999996</v>
+        <v>0.86439999999999995</v>
       </c>
       <c r="H19" s="5">
-        <v>120</v>
+        <v>20</v>
       </c>
       <c r="I19" s="5">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="J19" s="5">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="K19" s="5">
-        <v>125</v>
+        <v>31</v>
       </c>
       <c r="L19" s="9">
-        <v>0.81</v>
+        <v>0.86</v>
       </c>
       <c r="M19" s="9">
-        <v>0.86</v>
+        <v>0.91</v>
       </c>
       <c r="N19" s="9">
-        <v>0.84</v>
+        <v>0.89</v>
       </c>
       <c r="O19" s="11">
-        <v>0.88300000000000001</v>
+        <v>0.874</v>
       </c>
       <c r="P19" s="5">
-        <v>1744</v>
+        <v>1726</v>
       </c>
       <c r="Q19" s="5">
-        <v>217</v>
+        <v>235</v>
       </c>
       <c r="R19" s="5">
         <v>17</v>
@@ -2145,26 +2148,26 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="V19" s="9">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="W19" s="7">
-        <f t="shared" si="0"/>
-        <v>0.99034639409426461</v>
+        <f>P19/(P19+R19)</f>
+        <v>0.99024670109007462</v>
       </c>
       <c r="X19" s="7">
-        <f t="shared" si="1"/>
-        <v>0.8893421723610403</v>
+        <f>P19/(P19+Q19)</f>
+        <v>0.88016318204997446</v>
       </c>
       <c r="Y19" s="18">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Z19" s="7">
-        <f t="shared" si="2"/>
-        <v>0.10256410256410256</v>
+        <f>Y19/39</f>
+        <v>0.17948717948717949</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="5">
@@ -2231,23 +2234,23 @@
         <v>0.22</v>
       </c>
       <c r="W20" s="7">
-        <f t="shared" si="0"/>
+        <f>P20/(P20+R20)</f>
         <v>0.9897794513179129</v>
       </c>
       <c r="X20" s="7">
-        <f t="shared" si="1"/>
+        <f>P20/(P20+Q20)</f>
         <v>0.93829678735339117</v>
       </c>
       <c r="Y20" s="18">
         <v>9</v>
       </c>
       <c r="Z20" s="7">
-        <f t="shared" si="2"/>
+        <f>Y20/39</f>
         <v>0.23076923076923078</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="23" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="5">
@@ -2314,23 +2317,23 @@
         <v>0.18</v>
       </c>
       <c r="W21" s="7">
-        <f t="shared" si="0"/>
+        <f>P21/(P21+R21)</f>
         <v>0.98955470038482685</v>
       </c>
       <c r="X21" s="7">
-        <f t="shared" si="1"/>
+        <f>P21/(P21+Q21)</f>
         <v>0.91789903110657822</v>
       </c>
       <c r="Y21" s="18">
         <v>4</v>
       </c>
       <c r="Z21" s="7">
-        <f t="shared" si="2"/>
+        <f>Y21/39</f>
         <v>0.10256410256410256</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="23" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="5">
@@ -2397,23 +2400,23 @@
         <v>0.12</v>
       </c>
       <c r="W22" s="7">
-        <f t="shared" si="0"/>
+        <f>P22/(P22+R22)</f>
         <v>0.98830409356725146</v>
       </c>
       <c r="X22" s="7">
-        <f t="shared" si="1"/>
+        <f>P22/(P22+Q22)</f>
         <v>0.86180520142784289</v>
       </c>
       <c r="Y22" s="18">
         <v>3</v>
       </c>
       <c r="Z22" s="7">
-        <f t="shared" si="2"/>
+        <f>Y22/39</f>
         <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="5">
@@ -2480,23 +2483,23 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="W23" s="7">
-        <f t="shared" si="0"/>
+        <f>P23/(P23+R23)</f>
         <v>0.98687807545106621</v>
       </c>
       <c r="X23" s="7">
-        <f t="shared" si="1"/>
+        <f>P23/(P23+Q23)</f>
         <v>0.92044875063742992</v>
       </c>
       <c r="Y23" s="18">
         <v>1</v>
       </c>
       <c r="Z23" s="7">
-        <f t="shared" si="2"/>
+        <f>Y23/39</f>
         <v>2.564102564102564E-2</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="23" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="5">
@@ -2563,18 +2566,18 @@
         <v>0.19</v>
       </c>
       <c r="W24" s="7">
-        <f t="shared" si="0"/>
+        <f>P24/(P24+R24)</f>
         <v>0.98632298790110473</v>
       </c>
       <c r="X24" s="7">
-        <f t="shared" si="1"/>
+        <f>P24/(P24+Q24)</f>
         <v>0.95614482406935242</v>
       </c>
       <c r="Y24" s="18">
         <v>8</v>
       </c>
       <c r="Z24" s="7">
-        <f t="shared" si="2"/>
+        <f>Y24/39</f>
         <v>0.20512820512820512</v>
       </c>
     </row>
@@ -2646,18 +2649,18 @@
         <v>0.21</v>
       </c>
       <c r="W25" s="7">
-        <f t="shared" si="0"/>
+        <f>P25/(P25+R25)</f>
         <v>0.98597402597402595</v>
       </c>
       <c r="X25" s="7">
-        <f t="shared" si="1"/>
+        <f>P25/(P25+Q25)</f>
         <v>0.96787353391126973</v>
       </c>
       <c r="Y25" s="18">
         <v>8</v>
       </c>
       <c r="Z25" s="7">
-        <f t="shared" si="2"/>
+        <f>Y25/39</f>
         <v>0.20512820512820512</v>
       </c>
     </row>
@@ -2729,18 +2732,18 @@
         <v>0.2</v>
       </c>
       <c r="W26" s="7">
-        <f t="shared" si="0"/>
+        <f>P26/(P26+R26)</f>
         <v>0.98590814196242171</v>
       </c>
       <c r="X26" s="7">
-        <f t="shared" si="1"/>
+        <f>P26/(P26+Q26)</f>
         <v>0.96328403875573687</v>
       </c>
       <c r="Y26" s="18">
         <v>5</v>
       </c>
       <c r="Z26" s="7">
-        <f t="shared" si="2"/>
+        <f>Y26/39</f>
         <v>0.12820512820512819</v>
       </c>
     </row>
@@ -2751,8 +2754,8 @@
       <c r="B27" s="5">
         <v>0.25</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>22</v>
+      <c r="C27" s="5">
+        <v>7</v>
       </c>
       <c r="D27" s="5">
         <v>10</v>
@@ -2764,19 +2767,19 @@
         <v>16</v>
       </c>
       <c r="G27" s="11">
-        <v>0.98299999999999998</v>
+        <v>0.98499999999999999</v>
       </c>
       <c r="H27" s="5">
-        <v>5317</v>
+        <v>5550</v>
       </c>
       <c r="I27" s="5">
-        <v>138</v>
+        <v>111</v>
       </c>
       <c r="J27" s="5">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="K27" s="5">
-        <v>6102</v>
+        <v>6149</v>
       </c>
       <c r="L27" s="9">
         <v>0.98</v>
@@ -2785,16 +2788,16 @@
         <v>0.99</v>
       </c>
       <c r="N27" s="9">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
       <c r="O27" s="11">
-        <v>0.95450000000000002</v>
+        <v>0.95650000000000002</v>
       </c>
       <c r="P27" s="5">
-        <v>1898</v>
+        <v>1902</v>
       </c>
       <c r="Q27" s="5">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="R27" s="5">
         <v>28</v>
@@ -2803,28 +2806,25 @@
         <v>11</v>
       </c>
       <c r="T27" s="9">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="U27" s="9">
         <v>0.28000000000000003</v>
       </c>
       <c r="V27" s="9">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="W27" s="7">
-        <f t="shared" si="0"/>
-        <v>0.98546209761163028</v>
+        <f>P27/(P27+R27)</f>
+        <v>0.9854922279792746</v>
       </c>
       <c r="X27" s="7">
-        <f t="shared" si="1"/>
-        <v>0.96787353391126973</v>
-      </c>
-      <c r="Y27" s="18">
-        <v>8</v>
+        <f>P27/(P27+Q27)</f>
+        <v>0.96991330953595101</v>
       </c>
       <c r="Z27" s="7">
-        <f t="shared" si="2"/>
-        <v>0.20512820512820512</v>
+        <f>Y27/39</f>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -2834,11 +2834,11 @@
       <c r="B28" s="5">
         <v>0.25</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="5">
         <v>10</v>
-      </c>
-      <c r="D28" s="5">
-        <v>1000</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>17</v>
@@ -2847,37 +2847,37 @@
         <v>16</v>
       </c>
       <c r="G28" s="11">
-        <v>0.98550000000000004</v>
+        <v>0.98299999999999998</v>
       </c>
       <c r="H28" s="5">
-        <v>5522</v>
+        <v>5317</v>
       </c>
       <c r="I28" s="5">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J28" s="5">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="K28" s="5">
-        <v>6180</v>
+        <v>6102</v>
       </c>
       <c r="L28" s="9">
         <v>0.98</v>
       </c>
       <c r="M28" s="9">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="N28" s="9">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
       <c r="O28" s="11">
-        <v>0.95199999999999996</v>
+        <v>0.95450000000000002</v>
       </c>
       <c r="P28" s="5">
-        <v>1893</v>
+        <v>1898</v>
       </c>
       <c r="Q28" s="5">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="R28" s="5">
         <v>28</v>
@@ -2886,7 +2886,7 @@
         <v>11</v>
       </c>
       <c r="T28" s="9">
-        <v>0.14000000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="U28" s="9">
         <v>0.28000000000000003</v>
@@ -2895,19 +2895,19 @@
         <v>0.19</v>
       </c>
       <c r="W28" s="7">
-        <f t="shared" si="0"/>
-        <v>0.98542425819885471</v>
+        <f>P28/(P28+R28)</f>
+        <v>0.98546209761163028</v>
       </c>
       <c r="X28" s="7">
-        <f t="shared" si="1"/>
-        <v>0.96532381438041814</v>
+        <f>P28/(P28+Q28)</f>
+        <v>0.96787353391126973</v>
       </c>
       <c r="Y28" s="18">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Z28" s="7">
-        <f t="shared" si="2"/>
-        <v>0.15384615384615385</v>
+        <f>Y28/39</f>
+        <v>0.20512820512820512</v>
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -2917,8 +2917,8 @@
       <c r="B29" s="5">
         <v>0.25</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>22</v>
+      <c r="C29" s="5">
+        <v>10</v>
       </c>
       <c r="D29" s="5">
         <v>1000</v>
@@ -2930,19 +2930,19 @@
         <v>16</v>
       </c>
       <c r="G29" s="11">
-        <v>0.98570000000000002</v>
+        <v>0.98550000000000004</v>
       </c>
       <c r="H29" s="5">
-        <v>5313</v>
+        <v>5522</v>
       </c>
       <c r="I29" s="5">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J29" s="5">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="K29" s="5">
-        <v>6133</v>
+        <v>6180</v>
       </c>
       <c r="L29" s="9">
         <v>0.98</v>
@@ -2954,13 +2954,13 @@
         <v>0.99</v>
       </c>
       <c r="O29" s="11">
-        <v>0.95099999999999996</v>
+        <v>0.95199999999999996</v>
       </c>
       <c r="P29" s="5">
-        <v>1891</v>
+        <v>1893</v>
       </c>
       <c r="Q29" s="5">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="R29" s="5">
         <v>28</v>
@@ -2975,21 +2975,21 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="V29" s="9">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
       <c r="W29" s="7">
-        <f t="shared" si="0"/>
-        <v>0.98540906722251176</v>
+        <f>P29/(P29+R29)</f>
+        <v>0.98542425819885471</v>
       </c>
       <c r="X29" s="7">
-        <f t="shared" si="1"/>
-        <v>0.96430392656807751</v>
+        <f>P29/(P29+Q29)</f>
+        <v>0.96532381438041814</v>
       </c>
       <c r="Y29" s="18">
         <v>6</v>
       </c>
       <c r="Z29" s="7">
-        <f t="shared" si="2"/>
+        <f>Y29/39</f>
         <v>0.15384615384615385</v>
       </c>
     </row>
@@ -3004,46 +3004,46 @@
         <v>22</v>
       </c>
       <c r="D30" s="5">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G30" s="11">
-        <v>0.97755000000000003</v>
+        <v>0.98570000000000002</v>
       </c>
       <c r="H30" s="5">
-        <v>6349</v>
+        <v>5313</v>
       </c>
       <c r="I30" s="5">
-        <v>8</v>
+        <v>142</v>
       </c>
       <c r="J30" s="5">
-        <v>138</v>
+        <v>24</v>
       </c>
       <c r="K30" s="5">
-        <v>9</v>
+        <v>6133</v>
       </c>
       <c r="L30" s="9">
-        <v>0.53</v>
+        <v>0.98</v>
       </c>
       <c r="M30" s="9">
-        <v>0.06</v>
+        <v>1</v>
       </c>
       <c r="N30" s="9">
-        <v>0.11</v>
+        <v>0.99</v>
       </c>
       <c r="O30" s="11">
-        <v>0.87649999999999995</v>
+        <v>0.95099999999999996</v>
       </c>
       <c r="P30" s="5">
-        <v>1742</v>
+        <v>1891</v>
       </c>
       <c r="Q30" s="5">
-        <v>219</v>
+        <v>70</v>
       </c>
       <c r="R30" s="5">
         <v>28</v>
@@ -3052,28 +3052,28 @@
         <v>11</v>
       </c>
       <c r="T30" s="9">
-        <v>0.05</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="U30" s="9">
         <v>0.28000000000000003</v>
       </c>
       <c r="V30" s="9">
-        <v>0.08</v>
+        <v>0.18</v>
       </c>
       <c r="W30" s="7">
-        <f t="shared" si="0"/>
-        <v>0.98418079096045197</v>
+        <f>P30/(P30+R30)</f>
+        <v>0.98540906722251176</v>
       </c>
       <c r="X30" s="7">
-        <f t="shared" si="1"/>
-        <v>0.88832228454869966</v>
+        <f>P30/(P30+Q30)</f>
+        <v>0.96430392656807751</v>
       </c>
       <c r="Y30" s="18">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="Z30" s="7">
-        <f t="shared" si="2"/>
-        <v>2.564102564102564E-2</v>
+        <f>Y30/39</f>
+        <v>0.15384615384615385</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -3083,50 +3083,50 @@
       <c r="B31" s="5">
         <v>0.25</v>
       </c>
-      <c r="C31" s="5">
-        <v>7</v>
+      <c r="C31" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="D31" s="5">
         <v>10</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F31" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G31" s="11">
-        <v>0.98499999999999999</v>
+        <v>0.97755000000000003</v>
       </c>
       <c r="H31" s="5">
-        <v>5550</v>
+        <v>6349</v>
       </c>
       <c r="I31" s="5">
-        <v>111</v>
+        <v>8</v>
       </c>
       <c r="J31" s="5">
-        <v>68</v>
+        <v>138</v>
       </c>
       <c r="K31" s="5">
-        <v>6149</v>
+        <v>9</v>
       </c>
       <c r="L31" s="9">
-        <v>0.98</v>
+        <v>0.53</v>
       </c>
       <c r="M31" s="9">
-        <v>0.99</v>
+        <v>0.06</v>
       </c>
       <c r="N31" s="9">
-        <v>0.99</v>
+        <v>0.11</v>
       </c>
       <c r="O31" s="11">
-        <v>0.95650000000000002</v>
+        <v>0.87649999999999995</v>
       </c>
       <c r="P31" s="5">
-        <v>1902</v>
+        <v>1742</v>
       </c>
       <c r="Q31" s="5">
-        <v>59</v>
+        <v>219</v>
       </c>
       <c r="R31" s="5">
         <v>28</v>
@@ -3135,25 +3135,28 @@
         <v>11</v>
       </c>
       <c r="T31" s="9">
-        <v>0.16</v>
+        <v>0.05</v>
       </c>
       <c r="U31" s="9">
         <v>0.28000000000000003</v>
       </c>
       <c r="V31" s="9">
-        <v>0.2</v>
+        <v>0.08</v>
       </c>
       <c r="W31" s="7">
-        <f t="shared" si="0"/>
-        <v>0.9854922279792746</v>
+        <f>P31/(P31+R31)</f>
+        <v>0.98418079096045197</v>
       </c>
       <c r="X31" s="7">
-        <f t="shared" si="1"/>
-        <v>0.96991330953595101</v>
+        <f>P31/(P31+Q31)</f>
+        <v>0.88832228454869966</v>
+      </c>
+      <c r="Y31" s="18">
+        <v>1</v>
       </c>
       <c r="Z31" s="7">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>Y31/39</f>
+        <v>2.564102564102564E-2</v>
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -3224,18 +3227,18 @@
         <v>0.19</v>
       </c>
       <c r="W32" s="7">
-        <f t="shared" si="0"/>
+        <f>P32/(P32+R32)</f>
         <v>0.98500517063081694</v>
       </c>
       <c r="X32" s="7">
-        <f t="shared" si="1"/>
+        <f>P32/(P32+Q32)</f>
         <v>0.97144314125446196</v>
       </c>
       <c r="Y32" s="18">
         <v>7</v>
       </c>
       <c r="Z32" s="7">
-        <f t="shared" si="2"/>
+        <f>Y32/39</f>
         <v>0.17948717948717949</v>
       </c>
     </row>
@@ -3307,18 +3310,18 @@
         <v>0.17</v>
       </c>
       <c r="W33" s="7">
-        <f t="shared" si="0"/>
+        <f>P33/(P33+R33)</f>
         <v>0.98491155046826218</v>
       </c>
       <c r="X33" s="7">
-        <f t="shared" si="1"/>
+        <f>P33/(P33+Q33)</f>
         <v>0.96532381438041814</v>
       </c>
       <c r="Y33" s="18">
         <v>6</v>
       </c>
       <c r="Z33" s="7">
-        <f t="shared" si="2"/>
+        <f>Y33/39</f>
         <v>0.15384615384615385</v>
       </c>
     </row>
@@ -3390,18 +3393,18 @@
         <v>0.17</v>
       </c>
       <c r="W34" s="7">
-        <f t="shared" si="0"/>
+        <f>P34/(P34+R34)</f>
         <v>0.98405349794238683</v>
       </c>
       <c r="X34" s="7">
-        <f t="shared" si="1"/>
+        <f>P34/(P34+Q34)</f>
         <v>0.97552269250382462</v>
       </c>
       <c r="Y34" s="18">
         <v>6</v>
       </c>
       <c r="Z34" s="7">
-        <f t="shared" si="2"/>
+        <f>Y34/39</f>
         <v>0.15384615384615385</v>
       </c>
     </row>
@@ -3473,18 +3476,18 @@
         <v>0.18</v>
       </c>
       <c r="W35" s="7">
-        <f t="shared" si="0"/>
+        <f>P35/(P35+R35)</f>
         <v>0.98394380331159059</v>
       </c>
       <c r="X35" s="7">
-        <f t="shared" si="1"/>
+        <f>P35/(P35+Q35)</f>
         <v>0.98493219487694628</v>
       </c>
       <c r="Y35" s="18">
         <v>8</v>
       </c>
       <c r="Z35" s="7">
-        <f t="shared" si="2"/>
+        <f>Y35/39</f>
         <v>0.20512820512820512</v>
       </c>
     </row>
@@ -3556,18 +3559,18 @@
         <v>0.08</v>
       </c>
       <c r="W36" s="7">
-        <f t="shared" si="0"/>
+        <f>P36/(P36+R36)</f>
         <v>0.98288770053475938</v>
       </c>
       <c r="X36" s="7">
-        <f t="shared" si="1"/>
+        <f>P36/(P36+Q36)</f>
         <v>0.93727689954105053</v>
       </c>
       <c r="Y36" s="18">
         <v>2</v>
       </c>
       <c r="Z36" s="7">
-        <f t="shared" si="2"/>
+        <f>Y36/39</f>
         <v>5.128205128205128E-2</v>
       </c>
     </row>
@@ -3639,18 +3642,18 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="W37" s="7">
-        <f t="shared" si="0"/>
+        <f>P37/(P37+R37)</f>
         <v>0.98272357723577231</v>
       </c>
       <c r="X37" s="7">
-        <f t="shared" si="1"/>
+        <f>P37/(P37+Q37)</f>
         <v>0.9862315145334013</v>
       </c>
       <c r="Y37" s="18">
         <v>6</v>
       </c>
       <c r="Z37" s="7">
-        <f t="shared" si="2"/>
+        <f>Y37/39</f>
         <v>0.15384615384615385</v>
       </c>
     </row>
@@ -3722,18 +3725,18 @@
         <v>0.12</v>
       </c>
       <c r="W38" s="7">
-        <f t="shared" si="0"/>
+        <f>P38/(P38+R38)</f>
         <v>0.98224251648909178</v>
       </c>
       <c r="X38" s="7">
-        <f t="shared" si="1"/>
+        <f>P38/(P38+Q38)</f>
         <v>0.98725140234574194</v>
       </c>
       <c r="Y38" s="18">
         <v>5</v>
       </c>
       <c r="Z38" s="7">
-        <f t="shared" si="2"/>
+        <f>Y38/39</f>
         <v>0.12820512820512819</v>
       </c>
     </row>
@@ -3805,18 +3808,18 @@
         <v>0.1</v>
       </c>
       <c r="W39" s="7">
-        <f t="shared" si="0"/>
+        <f>P39/(P39+R39)</f>
         <v>0.9821428571428571</v>
       </c>
       <c r="X39" s="7">
-        <f t="shared" si="1"/>
+        <f>P39/(P39+Q39)</f>
         <v>0.98164201937786844</v>
       </c>
       <c r="Y39" s="18">
         <v>4</v>
       </c>
       <c r="Z39" s="7">
-        <f t="shared" si="2"/>
+        <f>Y39/39</f>
         <v>0.10256410256410256</v>
       </c>
     </row>
@@ -3888,18 +3891,18 @@
         <v>0</v>
       </c>
       <c r="W40" s="7">
-        <f t="shared" si="0"/>
+        <f>P40/(P40+R40)</f>
         <v>0.98017285205897309</v>
       </c>
       <c r="X40" s="7">
-        <f t="shared" si="1"/>
+        <f>P40/(P40+Q40)</f>
         <v>0.98317185109637939</v>
       </c>
       <c r="Y40" s="18">
         <v>1</v>
       </c>
       <c r="Z40" s="7">
-        <f t="shared" si="2"/>
+        <f>Y40/39</f>
         <v>2.564102564102564E-2</v>
       </c>
     </row>

</xml_diff>